<commit_message>
Super assistant planning updated
</commit_message>
<xml_diff>
--- a/super_assistants.xlsx
+++ b/super_assistants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alpha/switchdrive/ACT-TP/act-github/act-tp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unils-my.sharepoint.com/personal/alpha_diallo_unil_ch/Documents/ACT-TP/act-github/act-tp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0437B4-7DCF-964E-92BC-3A7F80418C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{28F1D76B-82B7-C149-B436-F6BCA6ABCAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDF2FAF3-2172-AF48-9FB7-72B1C56CBD33}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Week 2: System Software</t>
   </si>
@@ -100,6 +99,21 @@
   </si>
   <si>
     <t>Week 8: Midterm</t>
+  </si>
+  <si>
+    <t>Le cours s’est bien passé.Pour ce qui est des exercices:Ils ont l’air de s’être bien familiarisé avec intelliJ et il n’y a eu que très peu de questions relatives à la mise en place des outils.Pas mal de difficultés avec les inputs/output mais après quelques explications les étudiants semblent comprendre.Les étudiants ont du mal à passer de Python à Java. Ils perçoivent Java comme étant plus complexe et verbeux, même si cela résulte en une structure plus rigoureuse.En ce qui concerne les fonctions, cela semblent encore assez abstrait et ils ont du mal à en saisir l’utilité et l’importance dans la programmation.Comme les semaines précédentes, la majorité des étudiants ne sont là que pour les deux premières heures des exercices et il reste bien moins de monde ensuite.</t>
+  </si>
+  <si>
+    <t>Pour ma part, je trouve que les étudiants ont encore beaucoup de mal à démarrer avec la programmation. La bonne nouvelle c'est qu'ils sont, pour la plupart, à l'aise avec les premières notions présentées en cours (architecture, conversion, opérations sur des nombres binaires, représentation des nombres).Pour ce qui est de la programmation, beaucoup peinent à utiliser IntelliJ, à croire qu'ils n'ont pas suivi le guide de démarrage. En regardant les statistiques, on a 124 personnes qui ont ouvert le guide contre 214 qui ont regardé les slides du cours et 207 pour ce qui est des exercices.La semaine prochaine, on reviendra sur des notions de programmation de base (variables, input/output, conditions, chaînes de caractères) avant d'introduire les fonctions.Pour qu'ils puissent suivre, nous devons les encourager à faire les exercices basiques et avancés pendant et en dehors des séances de TPs. Il faut aussi qu'on les encourage à nous contacter par mail et à utiliser le forum.</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Le cours s'est bien passé, la session de réponses aux questions du forum au début du cours était nécessaire pour préparer le midterm au vu des questions posées. Concernant les exercices, c'était la série de consolidation et de mon point de vue les exercices des semaines précédentes semblaient bien assimilés, malgré qu'il ait fallu revenir sur les fonctions récursives qui sont un concept assez compliqué. Utiliser l'analogie de stack LIFO marche bien pour ça.</t>
+  </si>
+  <si>
+    <t>Le cours s’est bien passé, ils n’avaient pas trop de questions. Pour les exercices, ils commencent à réussir à bien prendre en main les choses, mais ça réante assez difficile en général pour eux de jongler entre le Java et le python étant donné les grosses différences syntaxiques existantes.C’est aussi parfois un peu compliqué de leur expliquer pourquoi Java est tel qu’il est et python ne l’est pas (typiquement le fait de devoir rajouter PSVM en Java…)</t>
   </si>
 </sst>
 </file>
@@ -256,7 +270,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -293,28 +307,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -329,7 +337,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -619,10 +630,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="Q7" sqref="Q7"/>
-      <selection pane="topRight" activeCell="K12" sqref="K12"/>
+      <selection pane="topRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -630,8 +641,8 @@
     <col min="1" max="2" width="4.83203125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
@@ -666,7 +677,7 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="18" t="s">
         <v>21</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -688,7 +699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="385" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="9"/>
       <c r="C2" s="12" t="s">
@@ -696,13 +707,13 @@
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
-      <c r="J2" s="21"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
       <c r="M2" s="14"/>
@@ -710,7 +721,7 @@
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
     </row>
-    <row r="3" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="381" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6">
         <v>8</v>
       </c>
@@ -720,23 +731,23 @@
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="15" t="s">
-        <v>19</v>
+      <c r="F3" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="14"/>
       <c r="I3" s="15"/>
-      <c r="J3" s="22"/>
+      <c r="J3" s="20"/>
       <c r="K3" s="16"/>
       <c r="L3" s="15"/>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="22"/>
+      <c r="N3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="14"/>
       <c r="O3" s="14"/>
       <c r="P3" s="14"/>
     </row>
-    <row r="4" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="384" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>12</v>
       </c>
@@ -748,18 +759,18 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
-      <c r="J4" s="22"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="16"/>
       <c r="L4" s="14"/>
       <c r="M4" s="16"/>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="14"/>
+      <c r="O4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="14"/>
       <c r="P4" s="14"/>
     </row>
     <row r="5" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.15">
@@ -775,20 +786,22 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="16"/>
       <c r="L5" s="14"/>
       <c r="M5" s="16"/>
       <c r="N5" s="14"/>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="14"/>
+      <c r="P5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="14"/>
-    </row>
-    <row r="6" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:16" ht="319" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>12</v>
       </c>
@@ -802,23 +815,21 @@
       <c r="G6" s="15"/>
       <c r="H6" s="17"/>
       <c r="I6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="J6" s="21"/>
       <c r="K6" s="16"/>
       <c r="L6" s="17"/>
       <c r="M6" s="16"/>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
-      <c r="P6" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="P6" s="14"/>
     </row>
     <row r="7" spans="1:16" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="15"/>
@@ -826,12 +837,12 @@
       <c r="G7" s="15"/>
       <c r="H7" s="17"/>
       <c r="I7" s="13"/>
-      <c r="J7" s="23"/>
+      <c r="J7" s="21"/>
       <c r="K7" s="16"/>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="15"/>
+      <c r="M7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="16"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
@@ -839,7 +850,7 @@
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="15"/>
@@ -848,11 +859,11 @@
       <c r="G8" s="15"/>
       <c r="H8" s="17"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="24" t="s">
+      <c r="J8" s="19"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="17"/>
       <c r="M8" s="16"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>

</xml_diff>